<commit_message>
Mystery Gift Codes Working
Dreams do come true (I dreamed I could merge successfully)
</commit_message>
<xml_diff>
--- a/dialogue.xlsx
+++ b/dialogue.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Armeen\Documents\decomps\pokeemerald-expansion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEDD7C8-F5E8-44CF-B6E9-3D8C1F3A5D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4BCBC6-C1AC-4969-883A-F8A98803B1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="25760" windowHeight="13840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barks" sheetId="1" r:id="rId1"/>
     <sheet name="Trainers" sheetId="2" r:id="rId2"/>
+    <sheet name="Television" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>"It's like, my head's numb, today…"</t>
   </si>
@@ -80,6 +81,27 @@
   </si>
   <si>
     <t>MC Mack lyric</t>
+  </si>
+  <si>
+    <t>FERN: Well, the trainers that are fighting - years ago they were huddled around a television, and watching, and wondering.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCULLY: …and if you think about it, this year's Tournament is really a global one. Red, from Kanto. Silver, from Johto. Trainers from Unova, and Aloha, and Galar. </t>
+  </si>
+  <si>
+    <t>SCULLY: On the scoreboard in Snowpoint Temple, it is $CURRENTTIME in the city of miracles, Snowpoint City. And a crowd of 29,139 just sitting in to see the only trainer in tournament</t>
+  </si>
+  <si>
+    <t>history to manuever four no-knock games, and she's done it four straight years. And now she's capped it: on her fourth no-knock victory, she made it a perfect match."</t>
+  </si>
+  <si>
+    <t>wow that doesn't work…sorry vin</t>
+  </si>
+  <si>
+    <t>SCULLY: …her Typhlosion uses Burn Blast, lands a critical hit on Gengar, and she has done it! If you have a trainer hat, throw it to the sky!</t>
+  </si>
+  <si>
+    <t>You think about the young kids from these regions, who are huddled around TVs with their families, watching this series. These trainers are inspiring the next wave of global talent.</t>
   </si>
 </sst>
 </file>
@@ -492,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B18DF9A-7710-4EBF-BA27-E71BBA23EDF6}">
   <dimension ref="B2:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -522,4 +544,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E79F37-C079-403D-A8E7-F9B903C47EA6}">
+  <dimension ref="B3:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>